<commit_message>
Geo and cost data added
</commit_message>
<xml_diff>
--- a/Digital twin energy system/_mvlv_transformers.xlsx
+++ b/Digital twin energy system/_mvlv_transformers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Zero-energy-system-builder\Digital twin energy system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86D21E5-ED02-49AD-9C75-10D7CA5951CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C834418-9033-406A-8848-DEF3439B71E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="552" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21588" yWindow="2292" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mvlv_transformers" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>currentsta</t>
   </si>
@@ -72,70 +72,7 @@
     <t>ycoord</t>
   </si>
   <si>
-    <t>functional</t>
-  </si>
-  <si>
-    <t>2008/03/07 00:00:00.000</t>
-  </si>
-  <si>
-    <t>onGroundSurface</t>
-  </si>
-  <si>
-    <t>Netstation</t>
-  </si>
-  <si>
-    <t>!elec!e_fl_station_lv!105130684</t>
-  </si>
-  <si>
-    <t>technischGebouw</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>tot100cm</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
     <t>laagspanning</t>
-  </si>
-  <si>
-    <t>1965/01/01 00:00:00.000</t>
-  </si>
-  <si>
-    <t>!elec!e_fl_station_lv!14812414</t>
-  </si>
-  <si>
-    <t>1967/01/01 00:00:00.000</t>
-  </si>
-  <si>
-    <t>!elec!e_fl_station_lv!14812566</t>
-  </si>
-  <si>
-    <t>1951/01/01 00:00:00.000</t>
-  </si>
-  <si>
-    <t>!elec!e_fl_station_lv!14812702</t>
-  </si>
-  <si>
-    <t>2017/09/19 00:00:00.000</t>
-  </si>
-  <si>
-    <t>!elec!e_fl_station_lv!5398176138999304886</t>
-  </si>
-  <si>
-    <t>2018/06/12 00:00:00.000</t>
-  </si>
-  <si>
-    <t>!elec!e_fl_station_lv!5585320551425695102</t>
-  </si>
-  <si>
-    <t>2020/01/01 00:00:00.000</t>
-  </si>
-  <si>
-    <t>!elec!e_fl_station_lv!6499541792496733204</t>
   </si>
   <si>
     <t>ID</t>
@@ -175,9 +112,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -495,7 +431,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -505,10 +441,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -551,332 +487,122 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>105130684</v>
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="M2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
       <c r="N2">
-        <v>5.0762988130998732</v>
+        <v>6.0190944141807057</v>
       </c>
       <c r="O2">
-        <v>51.54557425806523</v>
+        <v>52.114936346501352</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>14812414</v>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
       <c r="N3">
-        <v>5.077731394208012</v>
+        <v>6.0229394254281523</v>
       </c>
       <c r="O3">
-        <v>51.54440926286491</v>
+        <v>52.115607626483794</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>14812566</v>
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="M4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
-        <v>22</v>
-      </c>
       <c r="N4">
-        <v>5.0697513063416011</v>
+        <v>6.0402832261971282</v>
       </c>
       <c r="O4">
-        <v>51.545114024493479</v>
+        <v>52.139494297683321</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>14812702</v>
+      <c r="A5">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="M5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
       <c r="N5">
-        <v>5.0742392557572638</v>
+        <v>6.0193876162701558</v>
       </c>
       <c r="O5">
-        <v>51.54694016355527</v>
+        <v>52.115127805191477</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5.3981761389993001E+18</v>
+      <c r="A6">
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="M6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" t="s">
-        <v>22</v>
-      </c>
       <c r="N6">
-        <v>5.0773856720038726</v>
+        <v>6.026830866555076</v>
       </c>
       <c r="O6">
-        <v>51.547049010216242</v>
+        <v>52.107976599574407</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5.5853205514256896E+18</v>
+      <c r="A7">
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="M7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
       <c r="N7">
-        <v>5.0704518414700042</v>
+        <v>6.0391020907205579</v>
       </c>
       <c r="O7">
-        <v>51.54668157971448</v>
+        <v>52.13635049500931</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6.4995417924967301E+18</v>
+      <c r="A8">
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" t="s">
+      <c r="M8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" t="s">
-        <v>22</v>
-      </c>
       <c r="N8">
-        <v>5.0724700688298396</v>
+        <v>6.029240297128494</v>
       </c>
       <c r="O8">
-        <v>51.544970177047261</v>
+        <v>52.109459904116342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>